<commit_message>
Single card in ticker.py
</commit_message>
<xml_diff>
--- a/assets/Sample Portfolio.xlsx
+++ b/assets/Sample Portfolio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richard\PycharmProjects\dash\YT_Dash_Tutorial\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardwalker/PycharmProjects/Dash_Equity/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865E9E99-3ECF-4E74-845A-B4F753F18113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14550B7-80D0-184E-AD67-F2D6A99AD28B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E661D0D6-7F69-4E3F-B2E7-FF912045EE3B}"/>
+    <workbookView xWindow="3880" yWindow="-19580" windowWidth="28800" windowHeight="17500" xr2:uid="{E661D0D6-7F69-4E3F-B2E7-FF912045EE3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>ABMD</t>
   </si>
   <si>
-    <t>APD</t>
-  </si>
-  <si>
     <t>GOOGL</t>
   </si>
   <si>
@@ -51,42 +48,12 @@
     <t>AAPL</t>
   </si>
   <si>
-    <t>BL</t>
-  </si>
-  <si>
-    <t>DOCU</t>
-  </si>
-  <si>
-    <t>FLGT</t>
-  </si>
-  <si>
     <t>LRCX</t>
   </si>
   <si>
-    <t>NIO</t>
-  </si>
-  <si>
-    <t>NVAX</t>
-  </si>
-  <si>
-    <t>SWAV</t>
-  </si>
-  <si>
-    <t>SEDG</t>
-  </si>
-  <si>
-    <t>REAL</t>
-  </si>
-  <si>
-    <t>OLED</t>
-  </si>
-  <si>
     <t>V</t>
   </si>
   <si>
-    <t>ZM</t>
-  </si>
-  <si>
     <t>NVDA</t>
   </si>
   <si>
@@ -241,6 +208,39 @@
   </si>
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>ALB</t>
+  </si>
+  <si>
+    <t>CRM</t>
+  </si>
+  <si>
+    <t>TYL</t>
+  </si>
+  <si>
+    <t>TMO</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>INCY</t>
+  </si>
+  <si>
+    <t>SYK</t>
+  </si>
+  <si>
+    <t>TPR</t>
+  </si>
+  <si>
+    <t>NXPI</t>
+  </si>
+  <si>
+    <t>SNPS</t>
+  </si>
+  <si>
+    <t>SWKS</t>
   </si>
 </sst>
 </file>
@@ -595,461 +595,461 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E6">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E7">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E8">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E9">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E11">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E12">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E13">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E14">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E15">
         <v>161</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E16">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
         <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" t="s">
-        <v>26</v>
       </c>
       <c r="E17">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E18">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E19">
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E20">
         <f>INT(3100/401)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E21">
         <f>INT(2500/194.68)</f>
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E22">
         <f>INT(2000/150)</f>
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" t="s">
         <v>52</v>
-      </c>
-      <c r="D23" t="s">
-        <v>63</v>
       </c>
       <c r="E23">
         <f>INT(1800/55)</f>
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="D24" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E24">
         <f>INT(1600/73.7)</f>
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D25" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E25">
         <f>INT(1500/84.4)</f>
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E26">
         <v>4</v>

</xml_diff>